<commit_message>
mini project part two
</commit_message>
<xml_diff>
--- a/Pandas-Project/Mini-Project-Part-2/output/project_part_two.xlsx
+++ b/Pandas-Project/Mini-Project-Part-2/output/project_part_two.xlsx
@@ -28,159 +28,159 @@
     <t>% Recommend</t>
   </si>
   <si>
+    <t>Le Wagon</t>
+  </si>
+  <si>
+    <t>Base10 Academy</t>
+  </si>
+  <si>
+    <t>Fullstack Academy</t>
+  </si>
+  <si>
+    <t>Ruby On The Beach</t>
+  </si>
+  <si>
+    <t>Science to Data Science</t>
+  </si>
+  <si>
+    <t>The Data Incubator</t>
+  </si>
+  <si>
+    <t>devCodeCamp</t>
+  </si>
+  <si>
+    <t>Coder's Lab</t>
+  </si>
+  <si>
+    <t>DESIGNATION</t>
+  </si>
+  <si>
+    <t>Code Institute</t>
+  </si>
+  <si>
+    <t>AngelHack Education</t>
+  </si>
+  <si>
+    <t>Betamore</t>
+  </si>
+  <si>
+    <t>Academia de CÃ³digo</t>
+  </si>
+  <si>
+    <t>CodeCraft School</t>
+  </si>
+  <si>
+    <t>Stackademy</t>
+  </si>
+  <si>
+    <t>Founders &amp; Coders</t>
+  </si>
+  <si>
+    <t>Omaha Code School</t>
+  </si>
+  <si>
+    <t>Telegraph Academy</t>
+  </si>
+  <si>
+    <t>Eleven Fifty Academy</t>
+  </si>
+  <si>
+    <t>We Got Coders</t>
+  </si>
+  <si>
+    <t>Grand Circus</t>
+  </si>
+  <si>
+    <t>Dev League</t>
+  </si>
+  <si>
+    <t>Code Platoon</t>
+  </si>
+  <si>
+    <t>EHD Academy</t>
+  </si>
+  <si>
+    <t>BoiseCodeWorks</t>
+  </si>
+  <si>
+    <t>Coder Factory</t>
+  </si>
+  <si>
+    <t>DigitalCrafts</t>
+  </si>
+  <si>
+    <t>CODEcamp Charleston</t>
+  </si>
+  <si>
     <t>Big Nerd Ranch</t>
   </si>
   <si>
-    <t>Grand Circus</t>
-  </si>
-  <si>
-    <t>Eleven Fifty Academy</t>
+    <t>Codecademy Labs</t>
+  </si>
+  <si>
+    <t>Grace Hopper Academy</t>
+  </si>
+  <si>
+    <t>AcadGild</t>
+  </si>
+  <si>
+    <t>Coder Foundry</t>
+  </si>
+  <si>
+    <t>CodeMasters Academy</t>
+  </si>
+  <si>
+    <t>Claim Academy</t>
+  </si>
+  <si>
+    <t>Byte Academy</t>
   </si>
   <si>
     <t>Operation Spark</t>
   </si>
   <si>
-    <t>Fullstack Academy</t>
-  </si>
-  <si>
-    <t>Codecademy Labs</t>
-  </si>
-  <si>
     <t>Origin Code Academy</t>
   </si>
   <si>
+    <t>Austin Coding Academy</t>
+  </si>
+  <si>
+    <t>Code Union</t>
+  </si>
+  <si>
     <t>Code 42</t>
   </si>
   <si>
-    <t>We Got Coders</t>
-  </si>
-  <si>
-    <t>Science to Data Science</t>
-  </si>
-  <si>
-    <t>Code Union</t>
+    <t>Ladies Learning Code</t>
+  </si>
+  <si>
+    <t>Dev Academy</t>
+  </si>
+  <si>
+    <t>Makers Academy</t>
+  </si>
+  <si>
+    <t>SeedPaths</t>
   </si>
   <si>
     <t>LEARN Academy</t>
   </si>
   <si>
-    <t>Coder's Lab</t>
-  </si>
-  <si>
-    <t>DESIGNATION</t>
-  </si>
-  <si>
-    <t>Academia de CÃ³digo</t>
-  </si>
-  <si>
-    <t>Dev League</t>
-  </si>
-  <si>
-    <t>Le Wagon</t>
-  </si>
-  <si>
-    <t>SeedPaths</t>
-  </si>
-  <si>
-    <t>AngelHack Education</t>
-  </si>
-  <si>
-    <t>Stackademy</t>
-  </si>
-  <si>
-    <t>Coder Foundry</t>
-  </si>
-  <si>
-    <t>devCodeCamp</t>
-  </si>
-  <si>
-    <t>Claim Academy</t>
-  </si>
-  <si>
-    <t>Ruby On The Beach</t>
-  </si>
-  <si>
-    <t>CodeCraft School</t>
-  </si>
-  <si>
-    <t>Byte Academy</t>
-  </si>
-  <si>
-    <t>Ladies Learning Code</t>
-  </si>
-  <si>
-    <t>Betamore</t>
-  </si>
-  <si>
-    <t>Grace Hopper Academy</t>
-  </si>
-  <si>
-    <t>Founders &amp; Coders</t>
-  </si>
-  <si>
-    <t>BoiseCodeWorks</t>
-  </si>
-  <si>
-    <t>Omaha Code School</t>
-  </si>
-  <si>
-    <t>Makers Academy</t>
-  </si>
-  <si>
-    <t>Coder Factory</t>
-  </si>
-  <si>
-    <t>CODEcamp Charleston</t>
-  </si>
-  <si>
-    <t>Code Institute</t>
-  </si>
-  <si>
-    <t>CodeMasters Academy</t>
-  </si>
-  <si>
-    <t>AcadGild</t>
+    <t>CodeaCamp</t>
+  </si>
+  <si>
+    <t>Viking Code School</t>
   </si>
   <si>
     <t>Launch School (formerly Tealeaf Academy)</t>
   </si>
   <si>
-    <t>CodeaCamp</t>
-  </si>
-  <si>
-    <t>Telegraph Academy</t>
-  </si>
-  <si>
-    <t>Dev Academy</t>
-  </si>
-  <si>
-    <t>Base10 Academy</t>
+    <t>Microsoft Research Data Science Summer School</t>
   </si>
   <si>
     <t>codeU</t>
   </si>
   <si>
-    <t>EHD Academy</t>
-  </si>
-  <si>
-    <t>Code Platoon</t>
-  </si>
-  <si>
-    <t>Viking Code School</t>
-  </si>
-  <si>
-    <t>The Data Incubator</t>
-  </si>
-  <si>
-    <t>Austin Coding Academy</t>
-  </si>
-  <si>
-    <t>DigitalCrafts</t>
-  </si>
-  <si>
-    <t>Microsoft Research Data Science Summer School</t>
-  </si>
-  <si>
     <t>Turing</t>
   </si>
   <si>
@@ -217,18 +217,18 @@
     <t>The Firehose Project</t>
   </si>
   <si>
+    <t>DevMountain</t>
+  </si>
+  <si>
+    <t>Nashville Software School</t>
+  </si>
+  <si>
     <t>CareerFoundry</t>
   </si>
   <si>
     <t>Software Guild</t>
   </si>
   <si>
-    <t>Nashville Software School</t>
-  </si>
-  <si>
-    <t>DevMountain</t>
-  </si>
-  <si>
     <t>Launch Academy</t>
   </si>
   <si>
@@ -241,33 +241,33 @@
     <t>The Iron Yard</t>
   </si>
   <si>
+    <t>LAMP Camp</t>
+  </si>
+  <si>
+    <t>Skillcrush</t>
+  </si>
+  <si>
     <t>Lighthouse Labs</t>
   </si>
   <si>
+    <t>Rutgers Coding Bootcamp</t>
+  </si>
+  <si>
     <t>Sabio.la</t>
   </si>
   <si>
-    <t>Rutgers Coding Bootcamp</t>
-  </si>
-  <si>
-    <t>LAMP Camp</t>
-  </si>
-  <si>
-    <t>Skillcrush</t>
-  </si>
-  <si>
     <t>Anyone Can Learn To Code</t>
   </si>
   <si>
     <t>IronHack</t>
   </si>
   <si>
+    <t>CodeNinja</t>
+  </si>
+  <si>
     <t>Code Fellows</t>
   </si>
   <si>
-    <t>CodeNinja</t>
-  </si>
-  <si>
     <t>New York Code + Design Academy</t>
   </si>
   <si>
@@ -292,12 +292,12 @@
     <t>Codeup</t>
   </si>
   <si>
+    <t>Bitmaker Labs</t>
+  </si>
+  <si>
     <t>10x.org.il</t>
   </si>
   <si>
-    <t>Bitmaker Labs</t>
-  </si>
-  <si>
     <t>CodeCore Bootcamp</t>
   </si>
   <si>
@@ -313,103 +313,103 @@
     <t>Bloc.io</t>
   </si>
   <si>
+    <t>Wyncode</t>
+  </si>
+  <si>
+    <t>LearningFuze</t>
+  </si>
+  <si>
+    <t>Fire Bootcamp</t>
+  </si>
+  <si>
+    <t>HackerYou</t>
+  </si>
+  <si>
+    <t>4Geeks Academy</t>
+  </si>
+  <si>
+    <t>Digital House</t>
+  </si>
+  <si>
     <t>Devschool</t>
   </si>
   <si>
+    <t>Mobile Makers Academy</t>
+  </si>
+  <si>
+    <t>Codesmith</t>
+  </si>
+  <si>
     <t>RefactorU</t>
   </si>
   <si>
-    <t>Codesmith</t>
+    <t>Metis</t>
+  </si>
+  <si>
+    <t>Bit Bootcamp</t>
   </si>
   <si>
     <t>PDX Code Guild</t>
   </si>
   <si>
-    <t>4Geeks Academy</t>
-  </si>
-  <si>
-    <t>Wyncode</t>
-  </si>
-  <si>
-    <t>Fire Bootcamp</t>
-  </si>
-  <si>
-    <t>Bit Bootcamp</t>
-  </si>
-  <si>
     <t>Camp Code Away</t>
   </si>
   <si>
-    <t>Mobile Makers Academy</t>
-  </si>
-  <si>
-    <t>Metis</t>
-  </si>
-  <si>
-    <t>LearningFuze</t>
-  </si>
-  <si>
-    <t>Digital House</t>
-  </si>
-  <si>
-    <t>HackerYou</t>
+    <t>tradecraft</t>
+  </si>
+  <si>
+    <t>Zip Code Wilmington</t>
+  </si>
+  <si>
+    <t>Starter League</t>
   </si>
   <si>
     <t>Coding House</t>
   </si>
   <si>
+    <t>We Can Code IT</t>
+  </si>
+  <si>
     <t>V School</t>
   </si>
   <si>
-    <t>We Can Code IT</t>
-  </si>
-  <si>
-    <t>tradecraft</t>
-  </si>
-  <si>
-    <t>Zip Code Wilmington</t>
-  </si>
-  <si>
-    <t>Starter League</t>
-  </si>
-  <si>
     <t>Codify Academy</t>
   </si>
   <si>
+    <t>Code For Progress</t>
+  </si>
+  <si>
+    <t>World Tech Makers</t>
+  </si>
+  <si>
+    <t>DaVinci Coders</t>
+  </si>
+  <si>
+    <t>Alphappl</t>
+  </si>
+  <si>
+    <t>Academic Work Academy</t>
+  </si>
+  <si>
+    <t>Astro Code School</t>
+  </si>
+  <si>
+    <t>Atlanta Code</t>
+  </si>
+  <si>
+    <t>Data Science Dojo</t>
+  </si>
+  <si>
+    <t>Interface Web School</t>
+  </si>
+  <si>
     <t>Montana Code School</t>
   </si>
   <si>
-    <t>Alphappl</t>
-  </si>
-  <si>
-    <t>World Tech Makers</t>
-  </si>
-  <si>
-    <t>DaVinci Coders</t>
-  </si>
-  <si>
-    <t>Academic Work Academy</t>
-  </si>
-  <si>
-    <t>Atlanta Code</t>
-  </si>
-  <si>
     <t>TalentBuddy</t>
   </si>
   <si>
-    <t>Interface Web School</t>
-  </si>
-  <si>
     <t>Academy X</t>
-  </si>
-  <si>
-    <t>Astro Code School</t>
-  </si>
-  <si>
-    <t>Data Science Dojo</t>
-  </si>
-  <si>
-    <t>Code For Progress</t>
   </si>
   <si>
     <t>100.00%</t>
@@ -882,10 +882,10 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>132</v>
@@ -896,10 +896,10 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>132</v>
@@ -910,10 +910,10 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>132</v>
@@ -938,10 +938,10 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>132</v>
@@ -952,10 +952,10 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>132</v>
@@ -966,10 +966,10 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>132</v>
@@ -994,10 +994,10 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>132</v>
@@ -1036,10 +1036,10 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>132</v>
@@ -1050,10 +1050,10 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>132</v>
@@ -1078,10 +1078,10 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>132</v>
@@ -1092,10 +1092,10 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>132</v>
@@ -1106,10 +1106,10 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
@@ -1120,10 +1120,10 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
@@ -1134,10 +1134,10 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
         <v>132</v>
@@ -1148,10 +1148,10 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
         <v>132</v>
@@ -1162,10 +1162,10 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22" t="s">
         <v>132</v>
@@ -1176,10 +1176,10 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
         <v>132</v>
@@ -1190,10 +1190,10 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
         <v>132</v>
@@ -1204,10 +1204,10 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
         <v>132</v>
@@ -1218,10 +1218,10 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
         <v>132</v>
@@ -1232,10 +1232,10 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
         <v>132</v>
@@ -1246,10 +1246,10 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
         <v>132</v>
@@ -1260,10 +1260,10 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
         <v>132</v>
@@ -1274,10 +1274,10 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
         <v>132</v>
@@ -1288,10 +1288,10 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
         <v>132</v>
@@ -1302,10 +1302,10 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
         <v>132</v>
@@ -1330,10 +1330,10 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
         <v>132</v>
@@ -1344,10 +1344,10 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
         <v>132</v>
@@ -1358,10 +1358,10 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>132</v>
@@ -1400,10 +1400,10 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
         <v>132</v>
@@ -1428,10 +1428,10 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
         <v>132</v>
@@ -1442,10 +1442,10 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
         <v>132</v>
@@ -1456,10 +1456,10 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
         <v>132</v>
@@ -1470,10 +1470,10 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
         <v>132</v>
@@ -1484,10 +1484,10 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D45" t="s">
         <v>132</v>
@@ -1498,10 +1498,10 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
         <v>132</v>
@@ -1512,10 +1512,10 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" t="s">
         <v>132</v>
@@ -1526,10 +1526,10 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D48" t="s">
         <v>132</v>
@@ -1540,10 +1540,10 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
         <v>132</v>
@@ -1568,10 +1568,10 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" t="s">
         <v>132</v>
@@ -1764,10 +1764,10 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D65" t="s">
         <v>144</v>
@@ -1778,10 +1778,10 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C66">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D66" t="s">
         <v>144</v>
@@ -1974,10 +1974,10 @@
         <v>82</v>
       </c>
       <c r="B80">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C80">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D80" t="s">
         <v>149</v>
@@ -1988,10 +1988,10 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D81" t="s">
         <v>149</v>
@@ -2212,10 +2212,10 @@
         <v>99</v>
       </c>
       <c r="B97">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D97" t="s">
         <v>158</v>
@@ -2226,10 +2226,10 @@
         <v>100</v>
       </c>
       <c r="B98">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D98" t="s">
         <v>158</v>
@@ -2240,10 +2240,10 @@
         <v>101</v>
       </c>
       <c r="B99">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D99" t="s">
         <v>158</v>
@@ -2282,10 +2282,10 @@
         <v>104</v>
       </c>
       <c r="B102">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D102" t="s">
         <v>158</v>
@@ -2296,10 +2296,10 @@
         <v>105</v>
       </c>
       <c r="B103">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C103">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D103" t="s">
         <v>158</v>
@@ -2310,10 +2310,10 @@
         <v>106</v>
       </c>
       <c r="B104">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D104" t="s">
         <v>158</v>
@@ -2338,10 +2338,10 @@
         <v>108</v>
       </c>
       <c r="B106">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D106" t="s">
         <v>158</v>
@@ -2366,10 +2366,10 @@
         <v>110</v>
       </c>
       <c r="B108">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D108" t="s">
         <v>158</v>
@@ -2394,10 +2394,10 @@
         <v>112</v>
       </c>
       <c r="B110">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D110" t="s">
         <v>158</v>
@@ -2534,7 +2534,7 @@
         <v>122</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -2548,7 +2548,7 @@
         <v>123</v>
       </c>
       <c r="B121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C121">
         <v>0</v>

</xml_diff>